<commit_message>
Added Updated Cancer Crosswalk
</commit_message>
<xml_diff>
--- a/ML_RPA_UiPathCode_Process/Cancer Crosswalk.xlsx
+++ b/ML_RPA_UiPathCode_Process/Cancer Crosswalk.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://huroncg-my.sharepoint.com/personal/khirst_huronconsultinggroup_com/Documents/Desktop/RPA/VA Project/ML_RPA_Use_Cases/ML_RPA_UiPathCode_Process/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://huroncg-my.sharepoint.com/personal/khirst_huronconsultinggroup_com/Documents/Desktop/RPA/VA Project/ML_RPA_Use_Cases/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="8_{94D74047-659A-44CD-9B26-E5C8751BFCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDBDAD5B-933A-4E09-8B04-57CAF7DEDB07}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="8_{94D74047-659A-44CD-9B26-E5C8751BFCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFDCC384-CEA8-4E0F-BE82-0B2F768962C2}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7710" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{D1BD660C-3ABA-47D9-B6C9-7B11077B7DA9}"/>
+    <workbookView xWindow="-28800" yWindow="7830" windowWidth="14400" windowHeight="17400" firstSheet="7" activeTab="11" xr2:uid="{D1BD660C-3ABA-47D9-B6C9-7B11077B7DA9}"/>
   </bookViews>
   <sheets>
     <sheet name="INQ030" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,11 @@
     <sheet name="MCQ371D" sheetId="5" r:id="rId5"/>
     <sheet name="HUQ071" sheetId="6" r:id="rId6"/>
     <sheet name="HUQ051" sheetId="12" r:id="rId7"/>
-    <sheet name="OHQ033" sheetId="11" r:id="rId8"/>
-    <sheet name="MCQ092" sheetId="10" r:id="rId9"/>
-    <sheet name="SMQ020" sheetId="7" r:id="rId10"/>
-    <sheet name="DPQ040" sheetId="8" r:id="rId11"/>
-    <sheet name="PUQ110" sheetId="9" r:id="rId12"/>
+    <sheet name="OHQ033" sheetId="7" r:id="rId8"/>
+    <sheet name="MCQ092" sheetId="8" r:id="rId9"/>
+    <sheet name="SMQ020" sheetId="9" r:id="rId10"/>
+    <sheet name="DPQ040" sheetId="10" r:id="rId11"/>
+    <sheet name="PUQ110" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="37">
   <si>
     <t>Yes</t>
   </si>
@@ -82,7 +82,7 @@
     <t>A few times a week</t>
   </si>
   <si>
-    <t>Every day and/or night</t>
+    <t>Ever day and/or night</t>
   </si>
   <si>
     <t>Excellent</t>
@@ -130,6 +130,9 @@
     <t>Nearly every day</t>
   </si>
   <si>
+    <t>.</t>
+  </si>
+  <si>
     <t>None</t>
   </si>
   <si>
@@ -154,7 +157,7 @@
     <t>16 or more</t>
   </si>
   <si>
-    <t>.</t>
+    <t>Don’t Know</t>
   </si>
 </sst>
 </file>
@@ -178,7 +181,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -186,12 +189,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,7 +528,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -543,7 +558,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.75">
@@ -551,7 +566,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.75">
@@ -559,15 +574,15 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>5</v>
+      <c r="B6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -576,17 +591,79 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91281DB-4EBC-41BD-B401-4D59A4DCE021}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805B6E7C-AFB8-4CFD-8237-93E1AF6AAF97}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E823BED7-41F2-4E4E-9EE3-1F2D2EF885DB}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.75">
@@ -599,42 +676,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
         <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -642,19 +735,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EB9781-7F89-44C1-91B5-55180AC5944A}">
-  <dimension ref="A1:B8"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B0C6DD-7C50-4C21-8D43-16D18EF3747E}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -666,7 +755,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -674,7 +763,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -682,42 +771,26 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -725,79 +798,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79079BBA-05F2-427A-854D-5021DB0F6AE8}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892648C9-E0C7-4AB2-8489-AE4346922BF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9420DC13-9027-4AB9-BC29-684638DBB964}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -830,7 +836,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -858,7 +864,7 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.75">
@@ -866,15 +872,15 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9">
-        <v>8</v>
+      <c r="B9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -883,17 +889,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9CAA85-5CF1-4C9E-A56E-6E59883ABC9C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46158280-A7E1-492A-B28C-29FE590CB485}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.75">
@@ -957,7 +962,7 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.75">
@@ -965,15 +970,15 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
-        <v>9</v>
+      <c r="B10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -982,7 +987,133 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94599400-CBEF-4873-A3BF-20DAFE472CA5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42F504-8040-41D8-93A5-4D0FE04A9497}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5D75BF-DB28-4C85-B3BA-11B5AEE3F8BA}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855A85F8-9461-4A98-890A-8515834AA0C7}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -990,8 +1121,70 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A2CADE-25FD-4953-9151-4F2538EB0849}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1005,42 +1198,98 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
+      <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1048,18 +1297,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9428C1-77A7-4384-8E3D-98F45A81FAAA}">
-  <dimension ref="A1:B6"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6496823C-C4A7-447B-ADFA-5FBA45C92B1F}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.31640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.75">
@@ -1072,7 +1320,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1080,7 +1328,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1088,7 +1336,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1096,7 +1344,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1104,10 +1352,34 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1115,79 +1387,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A3F740D-5C28-489A-B7D7-2AA8A3D91F50}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA57E32-BA7B-4DB1-B818-AA9F27B1C077}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13663B1-C3D5-49B8-A0A4-C4B2AB59285F}">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1202,256 +1407,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5D353E-5520-48E7-9C4C-E4B7B75BCB02}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="60.31640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320E3038-6B97-4943-9483-9D978F1B8A76}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>